<commit_message>
Updated code: Fixed typo in description, Removed Wireless BOM file
</commit_message>
<xml_diff>
--- a/Components/FAIO_Multiplexer_BOM.xlsx
+++ b/Components/FAIO_Multiplexer_BOM.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\FAIO-2\FAIO_Multiplexer\Components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milad\Development\FAIO_Multiplexer\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323F78AE-71B3-40B9-B786-909EC7140767}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90971A6-D49D-4E2D-B733-4CC897031FE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11140" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAIO-Multiplexer USB" sheetId="1" r:id="rId1"/>
-    <sheet name="FAIO-Multiplexer Bluetooth" sheetId="2" r:id="rId2"/>
-    <sheet name="FAIO-Multiplexe XAC or Joystick" sheetId="3" r:id="rId3"/>
+    <sheet name="FAIO-Multiplexe XAC or Joystick" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
   <si>
     <t>Index</t>
   </si>
@@ -111,24 +112,6 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/2771/1528-1514-ND/</t>
-  </si>
-  <si>
-    <t>FEATHER M0 BLUEFRUIT LE</t>
-  </si>
-  <si>
-    <t>1528-1562-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/2995/1528-1562-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/2829/1528-1517-ND</t>
-  </si>
-  <si>
-    <t>FEATHER 32U4 BLUEFRUIT LOOSE HDR</t>
-  </si>
-  <si>
-    <t>1528-1517-ND</t>
   </si>
   <si>
     <t>ANALOG 2-AXIS THUMB JOYSTICK WIT</t>
@@ -561,19 +544,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.90625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.89453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.3671875" style="2" customWidth="1"/>
     <col min="3" max="4" width="24" style="2" customWidth="1"/>
     <col min="5" max="5" width="32" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.90625" style="2"/>
+    <col min="6" max="6" width="16.62890625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5234375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -679,20 +662,20 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7">
         <v>0.1</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -835,20 +818,20 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F13" s="7">
         <v>0.1</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -902,21 +885,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A2EBB79-64DA-4046-BB4C-7A9E04984D82}">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26580692-9036-487D-AC12-7E4F660F0F9A}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.90625" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" customWidth="1"/>
+    <col min="1" max="1" width="6.89453125" customWidth="1"/>
+    <col min="2" max="2" width="12.3671875" customWidth="1"/>
     <col min="3" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.62890625" customWidth="1"/>
+    <col min="7" max="7" width="16.5234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -953,20 +936,20 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2">
-        <v>2995</v>
+        <v>2771</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2">
-        <v>29.95</v>
+        <v>19.95</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1025,20 +1008,20 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7">
         <v>0.1</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1066,375 +1049,6 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="2">
-        <f>(F2*B2+F3*B3+F4*B4+F5*B5+F6*B6)</f>
-        <v>38.950000000000003</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2829</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="2">
-        <v>29.95</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2">
-        <v>2.95</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>2886</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="2">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="2">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="2">
-        <f>(F10*B10+F11*B11+F12*B12+F13*B13+F14*B14)</f>
-        <v>38.950000000000003</v>
-      </c>
-      <c r="H15" s="2"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{54DCDEF7-55E6-4D66-B894-BD702A3DCFA4}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{E41DE43C-EF19-40E9-AB59-5C08E9976EB2}"/>
-    <hyperlink ref="H6" r:id="rId3" xr:uid="{02FA6F36-D8D7-4B6B-A83C-7D527827EDA3}"/>
-    <hyperlink ref="H2" r:id="rId4" xr:uid="{D0531FA3-65AA-4786-B0F0-C70B85428592}"/>
-    <hyperlink ref="H11" r:id="rId5" xr:uid="{0F47E7CA-717D-48A8-AB7D-C053F03A91B7}"/>
-    <hyperlink ref="H12" r:id="rId6" xr:uid="{F5E32E96-E2E2-4B11-AD8C-76252EA44C31}"/>
-    <hyperlink ref="H14" r:id="rId7" xr:uid="{5E04054A-9650-4380-AAB4-3DB187100DDF}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{0F160FD1-FEB9-4B42-9A72-00182DF14A0A}"/>
-    <hyperlink ref="H13" r:id="rId9" xr:uid="{694AB5F4-FFAE-4B57-91AB-CABF5081DF06}"/>
-    <hyperlink ref="H5" r:id="rId10" xr:uid="{197FAFE4-2BD5-494C-9BB6-8C43D3C99E48}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26580692-9036-487D-AC12-7E4F660F0F9A}">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="6.90625" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" customWidth="1"/>
-    <col min="3" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2771</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2">
-        <v>19.95</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2.95</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>2886</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1442,20 +1056,20 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3">
         <v>512</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2">
         <v>5.95</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1466,20 +1080,20 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2">
         <v>0.49</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1490,20 +1104,20 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3">
         <v>61300511121</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F9" s="3">
         <v>0.25</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8">

</xml_diff>

<commit_message>
Updated BOM file for the new enclosure
</commit_message>
<xml_diff>
--- a/Components/FAIO_Multiplexer_BOM.xlsx
+++ b/Components/FAIO_Multiplexer_BOM.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Personal\FAIO_Multiplexer\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B60D31B-C9BA-4A2C-AD1E-0D519DEC4785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC155633-D37A-40C1-8D4F-28142073AE04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAIO-Multiplexer USB" sheetId="1" r:id="rId1"/>
-    <sheet name="FAIO-Multiplexe XAC or Joystick" sheetId="3" r:id="rId2"/>
+    <sheet name="FAIO_Multiplexer_BOM" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>Index</t>
   </si>
@@ -99,9 +99,6 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">Alternative </t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -114,27 +111,6 @@
     <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/2771/1528-1514-ND/</t>
   </si>
   <si>
-    <t>ANALOG 2-AXIS THUMB JOYSTICK WIT</t>
-  </si>
-  <si>
-    <t>1528-2124-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/adafruit-industries-llc/512/1528-2124-ND/</t>
-  </si>
-  <si>
-    <t>CONN HDR 5POS 0.1 GOLD PCB</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC051LFBN-RC/S7038-ND</t>
-  </si>
-  <si>
-    <t>PPPC051LFBN-RC</t>
-  </si>
-  <si>
-    <t>S7038-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/wurth-electronics-inc/61300511121/732-5318-ND</t>
   </si>
   <si>
@@ -156,23 +132,31 @@
     <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT470R/CF14JT470RCT-ND/1830342</t>
   </si>
   <si>
-    <t>36-4701-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	
-HEX NUT 0.245" STEEL 6-32</t>
-  </si>
-  <si>
-    <t>36-9309-ND</t>
-  </si>
-  <si>
-    <t>MACH SCREW PAN HEAD SLOTTED 6-32</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/keystone-electronics/4701/316272</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/keystone-electronics/9309/2746088</t>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/4687/4499296</t>
+  </si>
+  <si>
+    <t>HEX NUT 0.197" NYLON M2.5</t>
+  </si>
+  <si>
+    <t>36-4687-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/29334/1532988</t>
+  </si>
+  <si>
+    <t>MACH SCREW PAN SLOTTED M2.5X0.45</t>
+  </si>
+  <si>
+    <t>36-29334-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/2750/6612470</t>
+  </si>
+  <si>
+    <t>1528-1858-ND</t>
+  </si>
+  <si>
+    <t>BATTERY LITHIUM 3.7V 350MAH (Optional)</t>
   </si>
 </sst>
 </file>
@@ -232,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,7 +224,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -564,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -603,8 +586,8 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>23</v>
+      <c r="H1" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -683,21 +666,21 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="C5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6">
         <v>0.1</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8" t="s">
-        <v>40</v>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -723,262 +706,155 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8">
-      <c r="A7">
+    <row r="7" spans="1:8">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4687</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3">
+        <v>29334</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3">
+        <v>61300511121</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2750</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="3">
-        <v>4701</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="F10" s="3">
+        <v>6.95</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="F12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="3">
-        <v>9309</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="F9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="2">
-        <f>(F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8)</f>
-        <v>29.749999999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="C10" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2771</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="2">
-        <v>19.95</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>26</v>
+      <c r="G12" s="2">
+        <f>(F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8+F9*B9)</f>
+        <v>30.68</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="2">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2.95</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="2">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14">
-        <v>2886</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="2">
-        <v>4</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8" t="s">
-        <v>40</v>
-      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="2">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.8">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="3">
-        <v>4701</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="3"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="2">
-        <v>7</v>
-      </c>
-      <c r="B18" s="2">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="3">
-        <v>9309</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="F19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="2">
-        <f>(F12*B12+F13*B13+F14*B14+F15*B15+F16*B16+F17*B17+F18*B18)</f>
-        <v>29.749999999999996</v>
-      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="H18" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -986,19 +862,13 @@
     <hyperlink ref="H4" r:id="rId2" xr:uid="{4DD09F3D-A506-47D3-BF03-F8C2639A2EC6}"/>
     <hyperlink ref="H6" r:id="rId3" xr:uid="{2C556464-C685-40E6-A45E-F9C3C7227E0D}"/>
     <hyperlink ref="H2" r:id="rId4" xr:uid="{25D91ED2-B16F-4D51-9CD9-F9FA81ADFFBE}"/>
-    <hyperlink ref="H13" r:id="rId5" xr:uid="{9998E661-EE9D-476E-A924-9E844227F0A2}"/>
-    <hyperlink ref="H14" r:id="rId6" xr:uid="{EAD79C85-527B-4905-B423-A7FDCB04F2E9}"/>
-    <hyperlink ref="H16" r:id="rId7" xr:uid="{38D01619-2C1C-436F-A205-9F6DD827B7B7}"/>
-    <hyperlink ref="H12" r:id="rId8" xr:uid="{D3605EDB-2688-4299-9573-CAEE8EA4B512}"/>
-    <hyperlink ref="H5" r:id="rId9" xr:uid="{82506C20-C239-4702-A36E-1219C82BD241}"/>
-    <hyperlink ref="H15" r:id="rId10" xr:uid="{D8C2ADA3-C733-458F-97BE-09487D5D7BED}"/>
-    <hyperlink ref="H7" r:id="rId11" xr:uid="{0A4488C4-4F7A-465E-AFF2-22579CDA1B67}"/>
-    <hyperlink ref="H8" r:id="rId12" xr:uid="{37CBC969-744C-4621-B4DA-894C9335B84C}"/>
-    <hyperlink ref="H17" r:id="rId13" xr:uid="{6363769F-F368-432E-A128-7AAE4A10C89D}"/>
-    <hyperlink ref="H18" r:id="rId14" xr:uid="{7E10E204-B493-4169-8D07-42E929F3CBC4}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{82506C20-C239-4702-A36E-1219C82BD241}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{8C655621-8D17-4747-A7D6-CB22233B20EF}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{DD193624-F2CB-4752-9951-9D3BE0210D6B}"/>
+    <hyperlink ref="H8" r:id="rId8" xr:uid="{39FD1782-E582-417A-928D-30470C49702D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -1007,7 +877,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1042,8 +912,8 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>23</v>
+      <c r="H1" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1054,20 +924,20 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2">
         <v>2771</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2">
         <v>19.95</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1125,21 +995,21 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="C5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6">
         <v>0.1</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8" t="s">
-        <v>40</v>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1171,23 +1041,23 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="D7" s="3">
-        <v>512</v>
+        <v>4687</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F7" s="2">
-        <v>5.95</v>
+        <v>0.15</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1195,23 +1065,23 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="D8" s="3">
+        <v>29334</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2">
-        <v>0.49</v>
+        <v>0.22</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1222,20 +1092,20 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3">
         <v>61300511121</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3">
         <v>0.25</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8">
@@ -1243,48 +1113,34 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2750</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="3">
-        <v>4701</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="F10" s="3">
-        <v>0.1</v>
+        <v>6.95</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="3">
-        <v>9309</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.1</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2"/>
@@ -1296,8 +1152,8 @@
         <v>4</v>
       </c>
       <c r="G12" s="2">
-        <f>(F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8+F9*B9+F10*B10+F11*B11)</f>
-        <v>36.44</v>
+        <f>(F2*B2+F3*B3+F4*B4+F5*B5+F6*B6+F7*B7+F8*B8+F9*B9)</f>
+        <v>30.68</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -1306,11 +1162,11 @@
     <hyperlink ref="H3" r:id="rId1" xr:uid="{57593BEC-058F-413F-BED9-83DC0E75D9D6}"/>
     <hyperlink ref="H4" r:id="rId2" xr:uid="{1F568088-B2D8-4C98-8A5C-0ED7121636CE}"/>
     <hyperlink ref="H6" r:id="rId3" xr:uid="{6B8DF80A-B880-449A-8EF1-79B4EBB20C84}"/>
-    <hyperlink ref="H7" r:id="rId4" xr:uid="{54F1C1C9-22C9-4C0A-BA29-28E2F3AF5A8C}"/>
-    <hyperlink ref="H2" r:id="rId5" xr:uid="{EA0B6A2B-DA19-490D-8B0D-46E9302BE8BD}"/>
-    <hyperlink ref="H5" r:id="rId6" xr:uid="{66367906-F303-4B07-8370-9075B0C97275}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{F016C3DE-A437-4DD4-9A0B-98333100D30C}"/>
-    <hyperlink ref="H11" r:id="rId8" xr:uid="{968F35BD-243C-413A-B2AB-BB07F3FF35E9}"/>
+    <hyperlink ref="H2" r:id="rId4" xr:uid="{EA0B6A2B-DA19-490D-8B0D-46E9302BE8BD}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{66367906-F303-4B07-8370-9075B0C97275}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{F016C3DE-A437-4DD4-9A0B-98333100D30C}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{54F1C1C9-22C9-4C0A-BA29-28E2F3AF5A8C}"/>
+    <hyperlink ref="H8" r:id="rId8" xr:uid="{ACAAEB30-9AC4-4D84-8EC1-5CC33CBE655B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>